<commit_message>
update one candidates' cellphone number.
</commit_message>
<xml_diff>
--- a/data/2019坊新招聘候选人列表_ver1.0.xlsx
+++ b/data/2019坊新招聘候选人列表_ver1.0.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4E6831-F58E-4EFB-A60A-E13C03AF749D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 Q1" sheetId="1" r:id="rId1"/>
@@ -280,18 +281,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -307,7 +308,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -409,8 +410,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -687,37 +688,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.25" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="34.5703125" customWidth="1"/>
-    <col min="10" max="10" width="52.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="7.75" customWidth="1"/>
+    <col min="7" max="7" width="5.375" customWidth="1"/>
+    <col min="8" max="8" width="11.25" customWidth="1"/>
+    <col min="9" max="9" width="34.625" customWidth="1"/>
+    <col min="10" max="10" width="52.25" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="8.125" customWidth="1"/>
+    <col min="13" max="13" width="8.625" customWidth="1"/>
+    <col min="14" max="14" width="10.375" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="17" max="17" width="10" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="9.875" customWidth="1"/>
     <col min="20" max="20" width="31" customWidth="1"/>
-    <col min="21" max="21" width="121.140625" customWidth="1"/>
+    <col min="21" max="21" width="121.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16.5">
+    <row r="1" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -782,7 +783,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="33">
+    <row r="2" spans="1:21" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
@@ -841,7 +842,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="66">
+    <row r="3" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -898,7 +899,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="66">
+    <row r="4" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>50</v>
       </c>
@@ -955,7 +956,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="66">
+    <row r="5" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -1012,7 +1013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="66">
+    <row r="6" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="66">
+    <row r="7" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="66">
+    <row r="8" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1187,7 +1188,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="29.25" customHeight="1">
+    <row r="9" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>61</v>
       </c>
@@ -1240,7 +1241,7 @@
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
     </row>
-    <row r="10" spans="1:21" ht="36.75" customHeight="1">
+    <row r="10" spans="1:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>64</v>
       </c>
@@ -1293,7 +1294,7 @@
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
     </row>
-    <row r="11" spans="1:21" ht="49.5">
+    <row r="11" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>68</v>
       </c>
@@ -1306,7 +1307,9 @@
       <c r="D11" s="12">
         <v>43578</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>15901864668</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1353,13 +1356,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J6" r:id="rId2"/>
-    <hyperlink ref="J7" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="B3:B8" r:id="rId5" display="hubinglei@jijiangspace.com"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B3:B8" r:id="rId5" display="hubinglei@jijiangspace.com" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
1. appended one candidate
</commit_message>
<xml_diff>
--- a/data/2019坊新招聘候选人列表_ver1.0.xlsx
+++ b/data/2019坊新招聘候选人列表_ver1.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02.WPS_JUMP\wps_deco\JiJiangOperatorTools\jump-mail-reception\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\personal\best\publicgit\hr\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED32DB0-167A-456B-AD93-FB00948136D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="81">
   <si>
     <t>姓名</t>
   </si>
@@ -259,17 +260,37 @@
   </si>
   <si>
     <t>我们对您的作品集很感兴趣，尤其是类似中南/地块大平层等PDF中一些理解和说明我们比较认可。您方便将现有作品的CAD 以及 3Dmax原文件（无需所有设计产品，任选您最中意一款即可）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陈照明 </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhaoming3117@qq.com</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>室内设计</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -284,7 +305,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -294,6 +315,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -386,8 +414,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -664,34 +692,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.25" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="52.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="21.375" customWidth="1"/>
+    <col min="6" max="6" width="7.75" customWidth="1"/>
+    <col min="7" max="7" width="5.375" customWidth="1"/>
+    <col min="8" max="8" width="11.25" customWidth="1"/>
+    <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="52.25" customWidth="1"/>
     <col min="11" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.625" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.75" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="21" max="21" width="69.42578125" customWidth="1"/>
-    <col min="22" max="22" width="121.140625" customWidth="1"/>
-    <col min="23" max="23" width="39.42578125" customWidth="1"/>
+    <col min="20" max="20" width="19.375" customWidth="1"/>
+    <col min="21" max="21" width="69.375" customWidth="1"/>
+    <col min="22" max="22" width="121.125" customWidth="1"/>
+    <col min="23" max="23" width="39.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1230,7 +1259,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="66" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>55</v>
       </c>
@@ -1423,22 +1452,79 @@
         <v>35</v>
       </c>
     </row>
+    <row r="12" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="12">
+        <v>43583</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="1">
+        <v>33</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S12" s="1"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="J2" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="J6" r:id="rId7"/>
-    <hyperlink ref="B8" r:id="rId8"/>
-    <hyperlink ref="J7" r:id="rId9"/>
-    <hyperlink ref="B8" r:id="rId10"/>
-    <hyperlink ref="B10" r:id="rId11"/>
-    <hyperlink ref="B11" r:id="rId12"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B12" r:id="rId13" xr:uid="{83DF0437-24C8-451A-BE9E-27FA5E9763A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added candidate's cellphone information.
</commit_message>
<xml_diff>
--- a/data/2019坊新招聘候选人列表_ver1.0.xlsx
+++ b/data/2019坊新招聘候选人列表_ver1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\personal\best\publicgit\hr\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED32DB0-167A-456B-AD93-FB00948136D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA197AA9-83CE-433B-9A9B-3E74DB28693A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1385,7 +1385,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>63</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>76</v>
       </c>
@@ -1465,7 +1465,9 @@
       <c r="D12" s="12">
         <v>43583</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>18005602123</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
process confirm mail for 陈照明
</commit_message>
<xml_diff>
--- a/data/2019坊新招聘候选人列表_ver1.0.xlsx
+++ b/data/2019坊新招聘候选人列表_ver1.0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\personal\best\publicgit\hr\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02.WPS_JUMP\wps_deco\JiJiangOperatorTools\jump-mail-reception\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA197AA9-83CE-433B-9A9B-3E74DB28693A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="75">
   <si>
     <t>姓名</t>
   </si>
@@ -130,6 +129,9 @@
     <t>您投递的求职申请我们已经收到。我们将会在7日内完成对您简历的处理。感谢您对本职位的关注，我们将会尽快同您取得联系。</t>
   </si>
   <si>
+    <t>我们看了您的酷家乐作品集，想对您的作品做进一步的了解。您方便将现有作品的CAD 以及 3Dmax原文件发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
+  </si>
+  <si>
     <t>合作方式参考我们的合作流程。主要采用工作包的形式，完成工作包，支付对应价款。</t>
   </si>
   <si>
@@ -145,12 +147,18 @@
     <t>已收到</t>
   </si>
   <si>
+    <t>我们对您的作品集很感兴趣，尤其是类似中南/地块大平层等PDF中一些理解和说明我们比较认可。您方便将现有作品的CAD 以及 3Dmax原文件（无需所有设计产品，任选您最中意一款即可）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
+  </si>
+  <si>
     <t>周启民</t>
   </si>
   <si>
     <t>9+</t>
   </si>
   <si>
+    <t>我们发现您的作品集大多为大宅和别墅类，其中的一些设计点我们也比较认可。您方便将现有作品的CAD 以及 3Dmax原文件（现有作品集中任意一款也可，普通商品房作品尤佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
+  </si>
+  <si>
     <t>葛洋</t>
   </si>
   <si>
@@ -160,6 +168,9 @@
     <t>N/A</t>
   </si>
   <si>
+    <t>我们发现您的作品集大多豪宅和别墅类，其中的一些设计点我们也比较认可。您方便将现有作品的CAD 以及 3Dmax原文件（现有作品集中任意一款也可，普通商品房作品尤佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
+  </si>
+  <si>
     <t>丁艳</t>
   </si>
   <si>
@@ -172,6 +183,9 @@
     <t>拉钩网</t>
   </si>
   <si>
+    <t>我们看了您的简历，对您的工作经验比较感兴趣。但您的作品提供链接中无论是文案编辑，设计师还是作品中提到的软装、硬装设计师均未见到您的名字，请问方便将手中手中作品的CAD ， 3Dmax以及PS原文件（各选其一款即可，普通商品房作品尤佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
+  </si>
+  <si>
     <t>覃婷婷</t>
   </si>
   <si>
@@ -184,113 +198,66 @@
     <t>2019-04-28</t>
   </si>
   <si>
+    <t>我们看了您的简历，对您的工作经验比较感兴趣。但您的作品提供链接中效果图主要为实景拍摄，请问方便将手中手中作品的CAD ，3Dmax以及PS原文件（各选其一款即可，普通商品房作品尤佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
+  </si>
+  <si>
     <t>潘珂璐</t>
   </si>
   <si>
+    <t>我们看了您的简历作品，对您的工作经验比较感兴趣。由于您的作品中效果图主标注为实景拍摄，附的CAD图比较小，请问方便将手中手中作品的CAD ，3Dmax以及PS原文件（如果还能附上对该作品的理解则更佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
+  </si>
+  <si>
+    <t>陈蒙</t>
+  </si>
+  <si>
+    <t>zhongliansanguo@foxmail.com</t>
+  </si>
+  <si>
+    <t>中专</t>
+  </si>
+  <si>
+    <t>刘新</t>
+  </si>
+  <si>
+    <t>582641020@qq.com</t>
+  </si>
+  <si>
     <t>您好，潘珂璐先生/女士，我们看了您的简历作品，对您的工作经验比较感兴趣。由于您的作品中效果图主标注为实景拍摄，附的CAD图比较小，请问方便将手中手中作品的CAD ，3Dmax以及PS原文件（如果还能附上对该作品的理解则更佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
   </si>
   <si>
-    <t>陈蒙</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhongliansanguo@foxmail.com</t>
-  </si>
-  <si>
-    <t>中专</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>室内设计</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>已收到</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS直聘</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>刘新</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>582641020@qq.com</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>黄洪</t>
   </si>
   <si>
     <t>1264339765@qq.com</t>
   </si>
   <si>
-    <t>大专</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>室内设计, 国家注册高级设计师</t>
   </si>
   <si>
-    <t>建议面试</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>我们看了您的简历，对您的工作经验和能力比较感兴趣。但您的作品中主要为效果图，请您任意选取一家装案例。将其中一个房间的CAD图纸、3DMax一个场景（需要带窗，阳光投射效果）发至我们                              的邮箱（或者共享文件链接）。我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
   </si>
   <si>
-    <t>我们看了您的简历作品，对您的工作经验比较感兴趣。由于您的作品中效果图主标注为实景拍摄，附的CAD图比较小，请问方便将手中手中作品的CAD ，3Dmax以及PS原文件（如果还能附上对该作品的理解则更佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
-  </si>
-  <si>
-    <t>我们看了您的简历，对您的工作经验比较感兴趣。但您的作品提供链接中效果图主要为实景拍摄，请问方便将手中手中作品的CAD ，3Dmax以及PS原文件（各选其一款即可，普通商品房作品尤佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
-  </si>
-  <si>
-    <t>我们看了您的简历，对您的工作经验比较感兴趣。但您的作品提供链接中无论是文案编辑，设计师还是作品中提到的软装、硬装设计师均未见到您的名字，请问方便将手中手中作品的CAD ， 3Dmax以及PS原文件（各选其一款即可，普通商品房作品尤佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
-  </si>
-  <si>
-    <t>我们发现您的作品集大多豪宅和别墅类，其中的一些设计点我们也比较认可。您方便将现有作品的CAD 以及 3Dmax原文件（现有作品集中任意一款也可，普通商品房作品尤佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
-  </si>
-  <si>
-    <t>我们发现您的作品集大多为大宅和别墅类，其中的一些设计点我们也比较认可。您方便将现有作品的CAD 以及 3Dmax原文件（现有作品集中任意一款也可，普通商品房作品尤佳）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
-  </si>
-  <si>
-    <t>我们看了您的酷家乐作品集，想对您的作品做进一步的了解。您方便将现有作品的CAD 以及 3Dmax原文件发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
-  </si>
-  <si>
-    <t>我们对您的作品集很感兴趣，尤其是类似中南/地块大平层等PDF中一些理解和说明我们比较认可。您方便将现有作品的CAD 以及 3Dmax原文件（无需所有设计产品，任选您最中意一款即可）发至我们的邮箱（或者共享文件链接），我们期望更全面的理解您的设计能力后进一步和您联系，谢谢。</t>
-  </si>
-  <si>
     <t xml:space="preserve">陈照明 </t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>zhaoming3117@qq.com</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>10+</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>室内设计</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>尚未填写</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -305,7 +272,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -315,13 +282,6 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -414,8 +374,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -692,35 +652,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="28.25" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="13.75" customWidth="1"/>
-    <col min="5" max="5" width="21.375" customWidth="1"/>
-    <col min="6" max="6" width="7.75" customWidth="1"/>
-    <col min="7" max="7" width="5.375" customWidth="1"/>
-    <col min="8" max="8" width="11.25" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="52.25" customWidth="1"/>
+    <col min="10" max="10" width="52.28515625" customWidth="1"/>
     <col min="11" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15.625" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="13.75" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="20" max="20" width="19.375" customWidth="1"/>
-    <col min="21" max="21" width="69.375" customWidth="1"/>
-    <col min="22" max="22" width="121.125" customWidth="1"/>
-    <col min="23" max="23" width="39.375" customWidth="1"/>
+    <col min="20" max="20" width="19.42578125" customWidth="1"/>
+    <col min="21" max="21" width="69.42578125" customWidth="1"/>
+    <col min="22" max="22" width="121.140625" customWidth="1"/>
+    <col min="23" max="23" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -855,15 +815,15 @@
         <v>34</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>24</v>
@@ -878,19 +838,19 @@
         <v>18616951840</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1">
         <v>31</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>30</v>
@@ -920,15 +880,15 @@
         <v>34</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>24</v>
@@ -943,19 +903,19 @@
         <v>13774251570</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G4" s="1">
         <v>34</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>30</v>
@@ -985,27 +945,27 @@
         <v>34</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D5" s="12">
         <v>43561</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>26</v>
@@ -1014,13 +974,13 @@
         <v>28</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>30</v>
@@ -1050,21 +1010,21 @@
         <v>34</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D6" s="12">
         <v>43561</v>
@@ -1082,13 +1042,13 @@
         <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>31</v>
@@ -1117,21 +1077,21 @@
         <v>34</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="W6" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D7" s="12">
         <v>43561</v>
@@ -1149,19 +1109,19 @@
         <v>3</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="L7" s="7" t="s">
         <v>31</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>31</v>
@@ -1186,21 +1146,21 @@
         <v>34</v>
       </c>
       <c r="V7" s="10" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="W7" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D8" s="12">
         <v>43561</v>
@@ -1209,7 +1169,7 @@
         <v>17621065221</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1">
         <v>25</v>
@@ -1221,7 +1181,7 @@
         <v>28</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>30</v>
@@ -1234,7 +1194,7 @@
         <v>31</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>32</v>
@@ -1253,21 +1213,21 @@
         <v>34</v>
       </c>
       <c r="V8" s="10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="D9" s="12">
         <v>43578</v>
@@ -1276,7 +1236,7 @@
         <v>18701914478</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G9" s="1">
         <v>30</v>
@@ -1285,13 +1245,13 @@
         <v>3</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>31</v>
@@ -1316,21 +1276,21 @@
         <v>34</v>
       </c>
       <c r="V9" s="10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="W9" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D10" s="12">
         <v>43578</v>
@@ -1339,7 +1299,7 @@
         <v>17316360798</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" s="1">
         <v>26</v>
@@ -1348,13 +1308,13 @@
         <v>3</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L10" s="7" t="s">
         <v>31</v>
@@ -1379,18 +1339,18 @@
         <v>34</v>
       </c>
       <c r="V10" s="10" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="W10" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>25</v>
@@ -1402,7 +1362,7 @@
         <v>15901864668</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="G11" s="1">
         <v>33</v>
@@ -1411,13 +1371,13 @@
         <v>10</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L11" s="7" t="s">
         <v>31</v>
@@ -1437,7 +1397,7 @@
         <v>32</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="T11" s="5">
         <v>4</v>
@@ -1446,18 +1406,18 @@
         <v>34</v>
       </c>
       <c r="V11" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="W11" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>25</v>
@@ -1469,29 +1429,31 @@
         <v>18005602123</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="G12" s="1">
         <v>33</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="M12" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="N12" s="7" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="O12" s="7"/>
       <c r="P12" s="7" t="s">
@@ -1505,28 +1467,28 @@
       </c>
       <c r="S12" s="1"/>
       <c r="T12" s="5"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
+      <c r="U12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="V12" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="W12" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="J2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="J6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="J7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B12" r:id="rId13" xr:uid="{83DF0437-24C8-451A-BE9E-27FA5E9763A6}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId2"/>
+    <hyperlink ref="J6" r:id="rId3"/>
+    <hyperlink ref="J7" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B12" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 徐媛媛 and one's information
</commit_message>
<xml_diff>
--- a/data/2019坊新招聘候选人列表_ver1.0.xlsx
+++ b/data/2019坊新招聘候选人列表_ver1.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02.WPS_JUMP\wps_operation_tools\mail_automation\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\personal\best\publicgit\hr\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03E632F-45C4-4C74-93EC-676D1012EA6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="80">
   <si>
     <t>姓名</t>
   </si>
@@ -247,17 +248,37 @@
   </si>
   <si>
     <t>尚未填写</t>
+  </si>
+  <si>
+    <t>329304319@qq.com</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>本科</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>已收到，酷家乐效果图网络连接：https://yun.kujiale.com/design/3FO41MHL5TVQ/show?fromqrcode=true&amp;from=panoMp</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>徐媛媛</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -272,7 +293,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -282,6 +303,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -374,8 +402,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -652,35 +680,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I11" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.25" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="21.375" customWidth="1"/>
+    <col min="6" max="6" width="7.75" customWidth="1"/>
+    <col min="7" max="7" width="5.375" customWidth="1"/>
+    <col min="8" max="8" width="11.25" customWidth="1"/>
     <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="52.28515625" customWidth="1"/>
+    <col min="10" max="10" width="122.125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.625" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.75" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="20" max="20" width="19.42578125" customWidth="1"/>
-    <col min="21" max="21" width="69.42578125" customWidth="1"/>
-    <col min="22" max="22" width="121.140625" customWidth="1"/>
-    <col min="23" max="23" width="39.42578125" customWidth="1"/>
+    <col min="20" max="20" width="19.375" customWidth="1"/>
+    <col min="21" max="21" width="69.375" customWidth="1"/>
+    <col min="22" max="22" width="121.125" customWidth="1"/>
+    <col min="23" max="23" width="39.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1477,18 +1505,83 @@
         <v>74</v>
       </c>
     </row>
+    <row r="13" spans="1:23" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="12">
+        <v>43590</v>
+      </c>
+      <c r="E13" s="1">
+        <v>17765101962</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="1">
+        <v>33</v>
+      </c>
+      <c r="H13" s="4">
+        <v>10</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S13" s="1"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="V13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="W13" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="J2" r:id="rId2"/>
-    <hyperlink ref="J6" r:id="rId3"/>
-    <hyperlink ref="J7" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{37B2EBB0-E72D-43A2-B72C-CC5F00DCB3E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated 杨国庆 mail information.
</commit_message>
<xml_diff>
--- a/data/2019坊新招聘候选人列表_ver1.0.xlsx
+++ b/data/2019坊新招聘候选人列表_ver1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\personal\best\publicgit\hr\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F28FEE2-9616-4B23-8B44-B09463405097}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CFCE91-D58D-4FA9-BF4C-44CE4D6B1107}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="86">
   <si>
     <t>姓名</t>
   </si>
@@ -293,6 +293,10 @@
 https://720yun.com/t/10ejr0haka1?scene_id=26422402
 https://720yun.com/t/8b2jephwsv7?scene_id=16142182
 https://720yun.com/t/82ejtzwmef7?scene_id=14319608</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1210292810@qq.com</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -713,7 +717,7 @@
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1656,7 +1660,9 @@
       <c r="A15" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="C15" s="7" t="s">
         <v>25</v>
       </c>
@@ -1719,8 +1725,9 @@
     <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B13" r:id="rId9" xr:uid="{37B2EBB0-E72D-43A2-B72C-CC5F00DCB3E0}"/>
+    <hyperlink ref="B15" r:id="rId10" xr:uid="{8DD0DD46-F5C6-47A4-8362-FA6EC0B23869}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>